<commit_message>
Remove wrong line from BOM
</commit_message>
<xml_diff>
--- a/m52tu, m54 PnP/Rev 1.2/BOM m52tu-m54_rev1.2.xlsx
+++ b/m52tu, m54 PnP/Rev 1.2/BOM m52tu-m54_rev1.2.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pasi\Documents\GitHub\Speeduino-M5x-PCBs\m52tu, m54 PnP\Rev 1.2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\GitHub\Speeduino-M5x-PCBs\m52tu, m54 PnP\Rev 1.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B93BBF8-7179-4AB1-A7AD-24DE569E68A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8C5CB2-F0E2-4096-A29A-51E382383601}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4875" yWindow="1470" windowWidth="21600" windowHeight="12735" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1815" yWindow="1350" windowWidth="26985" windowHeight="14850" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VR" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -39,7 +41,7 @@
     <author>Pasi</author>
   </authors>
   <commentList>
-    <comment ref="G22" authorId="0" shapeId="0" xr:uid="{348B1A39-87FE-44F8-89F3-7FB2DA1115C0}">
+    <comment ref="G21" authorId="0" shapeId="0" xr:uid="{348B1A39-87FE-44F8-89F3-7FB2DA1115C0}">
       <text>
         <r>
           <rPr>
@@ -69,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="194">
   <si>
     <t>Value</t>
   </si>
@@ -95,9 +97,6 @@
     <t>1uF</t>
   </si>
   <si>
-    <t>10k</t>
-  </si>
-  <si>
     <t>Yageo</t>
   </si>
   <si>
@@ -146,9 +145,6 @@
     <t>Digikey import</t>
   </si>
   <si>
-    <t>R14,R15</t>
-  </si>
-  <si>
     <t>100k</t>
   </si>
   <si>
@@ -198,18 +194,6 @@
   </si>
   <si>
     <t>603-RC1206FR-072KL</t>
-  </si>
-  <si>
-    <t>RES SMD 10K OHM 1% 1/8W 0603</t>
-  </si>
-  <si>
-    <t>RC0603FR-0710KL</t>
-  </si>
-  <si>
-    <t>603-RC0603FR-0710KL</t>
-  </si>
-  <si>
-    <t>311-10.0KHRTR-ND</t>
   </si>
   <si>
     <t>RES SMD 100K OHM 5% 1/8W 1206</t>
@@ -962,7 +946,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1004,9 +988,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1073,60 +1054,60 @@
     </xf>
   </cellXfs>
   <cellStyles count="54">
-    <cellStyle name="Avattu hyperlinkki" xfId="1" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="17" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="19" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="21" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="23" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="25" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="27" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="29" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="31" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="33" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="35" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="37" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="39" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="41" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="45" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="49" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="51" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="53" builtinId="9" hidden="1"/>
-    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1466,10 +1447,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P34"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1489,10 +1470,10 @@
   <sheetData>
     <row r="1" spans="1:16" ht="26.25" thickBot="1">
       <c r="A1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1513,28 +1494,28 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="O1" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="P1" s="25" t="s">
         <v>23</v>
+      </c>
+      <c r="P1" s="24" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="16.5" thickBot="1">
@@ -1552,38 +1533,38 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="4"/>
-      <c r="O2" s="18" t="str">
-        <f t="shared" ref="O2:O20" si="0">IF(NOT(H2=""),A2&amp;","&amp;H2,"")</f>
+      <c r="O2" s="17" t="str">
+        <f t="shared" ref="O2:O19" si="0">IF(NOT(H2=""),A2&amp;","&amp;H2,"")</f>
         <v/>
       </c>
-      <c r="P2" s="23"/>
+      <c r="P2" s="22"/>
     </row>
     <row r="3" spans="1:16" ht="16.5" thickBot="1">
       <c r="A3" s="12">
-        <f t="shared" ref="A3:A11" si="1">LEN(B3)-LEN(SUBSTITUTE(B3,",",""))+1</f>
+        <f t="shared" ref="A3:A10" si="1">LEN(B3)-LEN(SUBSTITUTE(B3,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="I3" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J3" s="5">
         <v>0.1</v>
@@ -1592,20 +1573,20 @@
         <v>0.1</v>
       </c>
       <c r="L3" s="6">
-        <f t="shared" ref="L3:L17" si="2">J3*A3</f>
+        <f t="shared" ref="L3:L16" si="2">J3*A3</f>
         <v>0.1</v>
       </c>
       <c r="M3" s="6">
-        <f t="shared" ref="M3:M17" si="3">K3*A3</f>
+        <f t="shared" ref="M3:M16" si="3">K3*A3</f>
         <v>0.1</v>
       </c>
       <c r="N3" s="4"/>
-      <c r="O3" s="18" t="str">
+      <c r="O3" s="17" t="str">
         <f t="shared" si="0"/>
         <v>1,311-7.5KERTR-ND</v>
       </c>
-      <c r="P3" s="23" t="str">
-        <f t="shared" ref="P3:P8" si="4">IF(NOT(I3=""),I3&amp;"|"&amp;A3,"")</f>
+      <c r="P3" s="22" t="str">
+        <f t="shared" ref="P3:P7" si="4">IF(NOT(I3=""),I3&amp;"|"&amp;A3,"")</f>
         <v>603-RC1206JR-077K5L|1</v>
       </c>
     </row>
@@ -1615,26 +1596,26 @@
         <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="I4" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J4" s="5">
         <v>0.1</v>
@@ -1651,11 +1632,11 @@
         <v>0.8</v>
       </c>
       <c r="N4" s="4"/>
-      <c r="O4" s="18" t="str">
+      <c r="O4" s="17" t="str">
         <f t="shared" si="0"/>
         <v>8,YAG1341TR-ND</v>
       </c>
-      <c r="P4" s="23" t="str">
+      <c r="P4" s="22" t="str">
         <f t="shared" si="4"/>
         <v>603-RC1206JR-071KP|8</v>
       </c>
@@ -1666,26 +1647,26 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="J5" s="5">
         <v>0.1</v>
@@ -1702,11 +1683,11 @@
         <v>0.4</v>
       </c>
       <c r="N5" s="4"/>
-      <c r="O5" s="18" t="str">
+      <c r="O5" s="17" t="str">
         <f t="shared" si="0"/>
         <v>4,311-2.00KFRTR-ND</v>
       </c>
-      <c r="P5" s="23" t="str">
+      <c r="P5" s="22" t="str">
         <f t="shared" si="4"/>
         <v>603-RC1206FR-072KL|4</v>
       </c>
@@ -1714,29 +1695,29 @@
     <row r="6" spans="1:16" ht="16.5" thickBot="1">
       <c r="A6" s="12">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>25</v>
+        <v>94</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>45</v>
+      <c r="I6" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="J6" s="5">
         <v>0.1</v>
@@ -1746,48 +1727,48 @@
       </c>
       <c r="L6" s="6">
         <f t="shared" si="2"/>
-        <v>0.2</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="M6" s="6">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="N6" s="4"/>
-      <c r="O6" s="18" t="str">
+      <c r="O6" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>2,311-10.0KHRTR-ND</v>
-      </c>
-      <c r="P6" s="23" t="str">
+        <v>6,YAG3912CT-ND</v>
+      </c>
+      <c r="P6" s="22" t="str">
         <f t="shared" si="4"/>
-        <v>603-RC0603FR-0710KL|2</v>
+        <v>603-AC1206JR-07100KL|6</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="16.5" thickBot="1">
       <c r="A7" s="12">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>100</v>
+        <v>54</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="J7" s="5">
         <v>0.1</v>
@@ -1797,113 +1778,113 @@
       </c>
       <c r="L7" s="6">
         <f t="shared" si="2"/>
-        <v>0.60000000000000009</v>
+        <v>0.1</v>
       </c>
       <c r="M7" s="6">
         <f t="shared" si="3"/>
-        <v>0.60000000000000009</v>
+        <v>0.1</v>
       </c>
       <c r="N7" s="4"/>
-      <c r="O7" s="18" t="str">
+      <c r="O7" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>6,YAG3912CT-ND</v>
-      </c>
-      <c r="P7" s="23" t="str">
+        <v>1,311-4.7KGRCT-ND</v>
+      </c>
+      <c r="P7" s="22" t="str">
         <f t="shared" si="4"/>
-        <v>603-AC1206JR-07100KL|6</v>
+        <v>603-RC0603JR-074K7L|1</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="16.5" thickBot="1">
       <c r="A8" s="12">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0.32</v>
+      </c>
+      <c r="K8" s="5">
+        <v>0.37</v>
+      </c>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>1, PCE3875CT-ND</v>
+      </c>
+      <c r="P8" s="22"/>
+    </row>
+    <row r="9" spans="1:16" ht="16.5" thickBot="1">
+      <c r="A9" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="J8" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="K8" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="L8" s="6">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="M8" s="6">
-        <f t="shared" si="3"/>
-        <v>0.1</v>
-      </c>
-      <c r="N8" s="4"/>
-      <c r="O8" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>1,311-4.7KGRCT-ND</v>
-      </c>
-      <c r="P8" s="23" t="str">
-        <f t="shared" si="4"/>
-        <v>603-RC0603JR-074K7L|1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="16.5" thickBot="1">
-      <c r="A9" s="12">
-        <v>1</v>
-      </c>
       <c r="B9" s="4" t="s">
-        <v>184</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>188</v>
+        <v>7</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>187</v>
+        <v>8</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>186</v>
+        <v>50</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>189</v>
+        <v>52</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>51</v>
       </c>
       <c r="J9" s="5">
-        <v>0.32</v>
+        <v>0.1</v>
       </c>
       <c r="K9" s="5">
-        <v>0.37</v>
-      </c>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
+        <v>0.1</v>
+      </c>
+      <c r="L9" s="6">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="M9" s="6">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
       <c r="N9" s="4"/>
-      <c r="O9" s="18" t="str">
+      <c r="O9" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>1, PCE3875CT-ND</v>
-      </c>
-      <c r="P9" s="23"/>
+        <v>1,311-1963-1-ND</v>
+      </c>
+      <c r="P9" s="22" t="str">
+        <f>IF(NOT(I9=""),I9&amp;"|"&amp;A9,"")</f>
+        <v>603-CC126KKX7R9BB105|1</v>
+      </c>
     </row>
     <row r="10" spans="1:16" ht="16.5" thickBot="1">
       <c r="A10" s="12">
@@ -1911,368 +1892,368 @@
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>59</v>
+        <v>45</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>49</v>
       </c>
       <c r="I10" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="J10" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="K10" s="5">
+        <v>48</v>
+      </c>
+      <c r="J10" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="K10" s="26">
         <v>0.1</v>
       </c>
       <c r="L10" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="L10" si="5">J10*A10</f>
         <v>0.1</v>
       </c>
       <c r="M10" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="M10" si="6">K10*A10</f>
         <v>0.1</v>
       </c>
       <c r="N10" s="4"/>
-      <c r="O10" s="18" t="str">
+      <c r="O10" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>1,311-1963-1-ND</v>
-      </c>
-      <c r="P10" s="23" t="str">
-        <f>IF(NOT(I10=""),I10&amp;"|"&amp;A10,"")</f>
-        <v>603-CC126KKX7R9BB105|1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="16.5" thickBot="1">
+        <v>1,311-1174-1-ND</v>
+      </c>
+      <c r="P10" s="22" t="str">
+        <f t="shared" ref="P10" si="7">IF(NOT(I10=""),I10&amp;"|"&amp;A10,"")</f>
+        <v>603-CC206KRX7R9BB103|1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="17.25" customHeight="1" thickBot="1">
       <c r="A11" s="12">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" ref="A11" si="8">LEN(B11)-LEN(SUBSTITUTE(B11,",",""))+1</f>
+        <v>3</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>21</v>
+        <v>95</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>51</v>
+        <v>113</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="I11" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="J11" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="K11" s="27">
+        <v>80</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="I11" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="J11" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="K11" s="26">
         <v>0.1</v>
       </c>
       <c r="L11" s="6">
-        <f t="shared" ref="L11" si="5">J11*A11</f>
-        <v>0.1</v>
+        <f t="shared" si="2"/>
+        <v>0.30000000000000004</v>
       </c>
       <c r="M11" s="6">
-        <f t="shared" ref="M11" si="6">K11*A11</f>
-        <v>0.1</v>
+        <f t="shared" si="3"/>
+        <v>0.30000000000000004</v>
       </c>
       <c r="N11" s="4"/>
-      <c r="O11" s="18" t="str">
+      <c r="O11" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>1,311-1174-1-ND</v>
-      </c>
-      <c r="P11" s="23" t="str">
-        <f t="shared" ref="P11" si="7">IF(NOT(I11=""),I11&amp;"|"&amp;A11,"")</f>
-        <v>603-CC206KRX7R9BB103|1</v>
+        <v>3,1830-1079-1-ND</v>
+      </c>
+      <c r="P11" s="22" t="str">
+        <f t="shared" ref="P11:P19" si="9">IF(NOT(I11=""),I11&amp;"|"&amp;A11,"")</f>
+        <v>743-IN-S85ATG|3</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="17.25" customHeight="1" thickBot="1">
       <c r="A12" s="12">
-        <f t="shared" ref="A12" si="8">LEN(B12)-LEN(SUBSTITUTE(B12,",",""))+1</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>101</v>
+        <v>172</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>119</v>
+        <v>175</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>84</v>
+        <v>174</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H12" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="I12" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="J12" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="K12" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="L12" s="6">
+        <v>173</v>
+      </c>
+      <c r="H12" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="I12" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="J12" s="26">
+        <v>0.43</v>
+      </c>
+      <c r="K12" s="5">
+        <v>0.42</v>
+      </c>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="22"/>
+    </row>
+    <row r="13" spans="1:16" ht="16.5" thickBot="1">
+      <c r="A13" s="12">
+        <f t="shared" ref="A13:A14" si="10">LEN(B13)-LEN(SUBSTITUTE(B13,",",""))+1</f>
+        <v>3</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H13" s="25"/>
+      <c r="I13" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="J13" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="K13" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="L13" s="6">
         <f t="shared" si="2"/>
         <v>0.30000000000000004</v>
       </c>
-      <c r="M12" s="6">
+      <c r="M13" s="6">
         <f t="shared" si="3"/>
         <v>0.30000000000000004</v>
       </c>
-      <c r="N12" s="4"/>
-      <c r="O12" s="18" t="str">
+      <c r="N13" s="4"/>
+      <c r="O13" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>3,1830-1079-1-ND</v>
-      </c>
-      <c r="P12" s="23" t="str">
-        <f t="shared" ref="P12:P20" si="9">IF(NOT(I12=""),I12&amp;"|"&amp;A12,"")</f>
-        <v>743-IN-S85ATG|3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A13" s="12">
-        <v>1</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="H13" s="26" t="s">
-        <v>183</v>
-      </c>
-      <c r="I13" s="29" t="s">
-        <v>182</v>
-      </c>
-      <c r="J13" s="27">
-        <v>0.43</v>
-      </c>
-      <c r="K13" s="5">
-        <v>0.42</v>
-      </c>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="23"/>
+        <v/>
+      </c>
+      <c r="P13" s="22" t="str">
+        <f t="shared" si="9"/>
+        <v>583-FM4004W-W|3</v>
+      </c>
     </row>
     <row r="14" spans="1:16" ht="16.5" thickBot="1">
       <c r="A14" s="12">
-        <f t="shared" ref="A14:A15" si="10">LEN(B14)-LEN(SUBSTITUTE(B14,",",""))+1</f>
-        <v>3</v>
+        <f t="shared" si="10"/>
+        <v>2</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="H14" s="26"/>
-      <c r="I14" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="J14" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="K14" s="27">
-        <v>0.1</v>
+      <c r="H14" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="I14" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="J14" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="K14" s="5">
+        <v>0.96</v>
       </c>
       <c r="L14" s="6">
         <f t="shared" si="2"/>
-        <v>0.30000000000000004</v>
+        <v>0.2</v>
       </c>
       <c r="M14" s="6">
         <f t="shared" si="3"/>
-        <v>0.30000000000000004</v>
+        <v>1.92</v>
       </c>
       <c r="N14" s="4"/>
-      <c r="O14" s="18" t="str">
+      <c r="O14" s="17" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="P14" s="23" t="str">
+        <v>2,NCV8403BDTRKGOSCT-NDD</v>
+      </c>
+      <c r="P14" s="22" t="str">
         <f t="shared" si="9"/>
-        <v>583-FM4004W-W|3</v>
+        <v>863-NCV8408DTRKG|2</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="16.5" thickBot="1">
       <c r="A15" s="12">
-        <f t="shared" si="10"/>
-        <v>2</v>
+        <f t="shared" ref="A15:A16" si="11">LEN(B15)-LEN(SUBSTITUTE(B15,",",""))+1</f>
+        <v>1</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="H15" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="I15" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="J15" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="K15" s="5">
-        <v>0.96</v>
+        <v>86</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="I15" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="J15" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="K15" s="26">
+        <v>0.1</v>
       </c>
       <c r="L15" s="6">
         <f t="shared" si="2"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="M15" s="6">
         <f t="shared" si="3"/>
-        <v>1.92</v>
+        <v>0.1</v>
       </c>
       <c r="N15" s="4"/>
-      <c r="O15" s="18" t="str">
+      <c r="O15" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>2,NCV8403BDTRKGOSCT-NDD</v>
-      </c>
-      <c r="P15" s="23" t="str">
+        <v>1,507-2450-1-ND</v>
+      </c>
+      <c r="P15" s="22" t="str">
         <f t="shared" si="9"/>
-        <v>863-NCV8408DTRKG|2</v>
+        <v>530-0685P5000-01|1</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="16.5" thickBot="1">
       <c r="A16" s="12">
-        <f t="shared" ref="A16:A17" si="11">LEN(B16)-LEN(SUBSTITUTE(B16,",",""))+1</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E16" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="19"/>
       <c r="F16" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="H16" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="I16" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="J16" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="K16" s="27">
-        <v>0.1</v>
+        <v>63</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="J16" s="5">
+        <v>1.94</v>
+      </c>
+      <c r="K16" s="5">
+        <v>1.94</v>
       </c>
       <c r="L16" s="6">
         <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>1.94</v>
       </c>
       <c r="M16" s="6">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>1.94</v>
       </c>
       <c r="N16" s="4"/>
-      <c r="O16" s="18" t="str">
+      <c r="O16" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>1,507-2450-1-ND</v>
-      </c>
-      <c r="P16" s="23" t="str">
+        <v>1, MMBT2222ALT1GOSCT-ND</v>
+      </c>
+      <c r="P16" s="22" t="str">
         <f t="shared" si="9"/>
-        <v>530-0685P5000-01|1</v>
+        <v>863-MMBT2222ALT1G|1</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="16.5" thickBot="1">
       <c r="A17" s="12">
-        <f t="shared" si="11"/>
-        <v>1</v>
+        <f t="shared" ref="A17:A19" si="12">LEN(B17)-LEN(SUBSTITUTE(B17,",",""))+1</f>
+        <v>6</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="E17" s="20"/>
-      <c r="F17" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>198</v>
+        <v>27</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>60</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>199</v>
+        <v>62</v>
       </c>
       <c r="J17" s="5">
         <v>1.94</v>
@@ -2281,100 +2262,100 @@
         <v>1.94</v>
       </c>
       <c r="L17" s="6">
-        <f t="shared" si="2"/>
-        <v>1.94</v>
+        <f t="shared" ref="L17:L20" si="13">J17*A17</f>
+        <v>11.64</v>
       </c>
       <c r="M17" s="6">
-        <f t="shared" si="3"/>
-        <v>1.94</v>
+        <f t="shared" ref="M17:M20" si="14">K17*A17</f>
+        <v>11.64</v>
       </c>
       <c r="N17" s="4"/>
-      <c r="O17" s="18" t="str">
+      <c r="O17" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>1, MMBT2222ALT1GOSCT-ND</v>
-      </c>
-      <c r="P17" s="23" t="str">
+        <v>6,ISL9V3040S3STCT-ND</v>
+      </c>
+      <c r="P17" s="22" t="str">
         <f t="shared" si="9"/>
-        <v>863-MMBT2222ALT1G|1</v>
+        <v>512-ISL9V3040S3ST|6</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="16.5" thickBot="1">
       <c r="A18" s="12">
-        <f t="shared" ref="A17:A20" si="12">LEN(B18)-LEN(SUBSTITUTE(B18,",",""))+1</f>
-        <v>6</v>
+        <f t="shared" si="12"/>
+        <v>2</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>70</v>
+        <v>107</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="E18" s="3"/>
-      <c r="F18" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="G18" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="H18" s="17" t="s">
-        <v>66</v>
+      <c r="F18" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="J18" s="5">
-        <v>1.94</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="K18" s="5">
-        <v>1.94</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="L18" s="6">
-        <f t="shared" ref="L17:L21" si="13">J18*A18</f>
-        <v>11.64</v>
+        <f t="shared" si="13"/>
+        <v>0.28000000000000003</v>
       </c>
       <c r="M18" s="6">
-        <f t="shared" ref="M17:M21" si="14">K18*A18</f>
-        <v>11.64</v>
+        <f t="shared" si="14"/>
+        <v>0.28000000000000003</v>
       </c>
       <c r="N18" s="4"/>
-      <c r="O18" s="18" t="str">
+      <c r="O18" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>6,ISL9V3040S3STCT-ND</v>
-      </c>
-      <c r="P18" s="23" t="str">
+        <v>2,497-14323-1-ND</v>
+      </c>
+      <c r="P18" s="22" t="str">
         <f t="shared" si="9"/>
-        <v>512-ISL9V3040S3ST|6</v>
+        <v>511-VNLD5090TR-E|2</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="16.5" thickBot="1">
       <c r="A19" s="12">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="E19" s="3"/>
-      <c r="F19" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G19" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>83</v>
+      <c r="F19" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>70</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="J19" s="5">
         <v>0.14000000000000001</v>
@@ -2384,600 +2365,549 @@
       </c>
       <c r="L19" s="6">
         <f t="shared" si="13"/>
-        <v>0.28000000000000003</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="M19" s="6">
         <f t="shared" si="14"/>
-        <v>0.28000000000000003</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="N19" s="4"/>
-      <c r="O19" s="18" t="str">
+      <c r="O19" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>2,497-14323-1-ND</v>
-      </c>
-      <c r="P19" s="23" t="str">
+        <v>1,MCP2551T-I/SNCT-ND</v>
+      </c>
+      <c r="P19" s="22" t="str">
         <f t="shared" si="9"/>
-        <v>511-VNLD5090TR-E|2</v>
+        <v>579-MCP2551T-I/SN|1</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="16.5" thickBot="1">
       <c r="A20" s="12">
-        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>71</v>
+        <v>165</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>114</v>
+        <v>168</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>73</v>
+        <v>169</v>
       </c>
       <c r="E20" s="3"/>
-      <c r="F20" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="G20" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>75</v>
+      <c r="F20" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="G20" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>170</v>
       </c>
       <c r="J20" s="5">
-        <v>0.14000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="K20" s="5">
-        <v>0.14000000000000001</v>
+        <v>1.59</v>
       </c>
       <c r="L20" s="6">
         <f t="shared" si="13"/>
-        <v>0.14000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="M20" s="6">
         <f t="shared" si="14"/>
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="N20" s="4"/>
-      <c r="O20" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1,MCP2551T-I/SNCT-ND</v>
-      </c>
-      <c r="P20" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>579-MCP2551T-I/SN|1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="16.5" thickBot="1">
+        <v>1.59</v>
+      </c>
+      <c r="N20" s="17"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="22"/>
+    </row>
+    <row r="21" spans="1:16" ht="26.25" thickBot="1">
       <c r="A21" s="12">
         <v>1</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>171</v>
+        <v>104</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>174</v>
+        <v>105</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>175</v>
+        <v>106</v>
       </c>
       <c r="E21" s="3"/>
-      <c r="F21" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="G21" s="35" t="s">
-        <v>172</v>
-      </c>
-      <c r="H21" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="I21" s="17" t="s">
-        <v>176</v>
+      <c r="F21" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>115</v>
       </c>
       <c r="J21" s="5">
-        <v>1.6</v>
+        <v>19</v>
       </c>
       <c r="K21" s="5">
-        <v>1.59</v>
+        <v>18</v>
       </c>
       <c r="L21" s="6">
-        <f t="shared" si="13"/>
-        <v>1.6</v>
+        <f t="shared" ref="L21:L27" si="15">J21*A21</f>
+        <v>19</v>
       </c>
       <c r="M21" s="6">
-        <f t="shared" si="14"/>
-        <v>1.59</v>
-      </c>
-      <c r="N21" s="18"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="23"/>
-    </row>
-    <row r="22" spans="1:16" ht="26.25" thickBot="1">
+        <f t="shared" ref="M21:M27" si="16">K21*A21</f>
+        <v>18</v>
+      </c>
+      <c r="N21" s="17"/>
+      <c r="O21" s="23" t="str">
+        <f t="shared" ref="O21:O26" si="17">IF(NOT(H21=""),A21&amp;","&amp;H21,"")</f>
+        <v>1,MPXA4250AC6U-ND</v>
+      </c>
+      <c r="P21" s="22" t="str">
+        <f t="shared" ref="P21:P26" si="18">IF(NOT(I21=""),I21&amp;"|"&amp;A21,"")</f>
+        <v>841-MPXA4250AC6U|1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="16.5" thickBot="1">
       <c r="A22" s="12">
         <v>1</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>111</v>
+      <c r="B22" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>146</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="E22" s="3"/>
-      <c r="F22" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="G22" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="H22" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="I22" s="17" t="s">
-        <v>121</v>
+      <c r="F22" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>144</v>
       </c>
       <c r="J22" s="5">
-        <v>19</v>
+        <v>13.82</v>
       </c>
       <c r="K22" s="5">
-        <v>18</v>
+        <v>13.8</v>
       </c>
       <c r="L22" s="6">
-        <f t="shared" ref="L22:L28" si="15">J22*A22</f>
-        <v>19</v>
+        <f t="shared" si="15"/>
+        <v>13.82</v>
       </c>
       <c r="M22" s="6">
-        <f t="shared" ref="M22:M28" si="16">K22*A22</f>
-        <v>18</v>
-      </c>
-      <c r="N22" s="18"/>
-      <c r="O22" s="24" t="str">
-        <f t="shared" ref="O22:O27" si="17">IF(NOT(H22=""),A22&amp;","&amp;H22,"")</f>
-        <v>1,MPXA4250AC6U-ND</v>
-      </c>
-      <c r="P22" s="23" t="str">
-        <f t="shared" ref="P22:P27" si="18">IF(NOT(I22=""),I22&amp;"|"&amp;A22,"")</f>
-        <v>841-MPXA4250AC6U|1</v>
+        <f t="shared" si="16"/>
+        <v>13.8</v>
+      </c>
+      <c r="N22" s="17"/>
+      <c r="O22" s="23" t="str">
+        <f t="shared" si="17"/>
+        <v>1,A123185-ND</v>
+      </c>
+      <c r="P22" s="22" t="str">
+        <f t="shared" si="18"/>
+        <v>571-7-967288-1|1</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="16.5" thickBot="1">
       <c r="A23" s="12">
         <v>1</v>
       </c>
-      <c r="B23" s="30" t="s">
-        <v>146</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>152</v>
+      <c r="B23" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>186</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>149</v>
+        <v>187</v>
       </c>
       <c r="E23" s="3"/>
-      <c r="F23" s="31" t="s">
-        <v>147</v>
-      </c>
-      <c r="G23" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="H23" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="I23" s="17" t="s">
-        <v>150</v>
+      <c r="F23" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>190</v>
       </c>
       <c r="J23" s="5">
-        <v>13.82</v>
+        <v>1.31</v>
       </c>
       <c r="K23" s="5">
-        <v>13.8</v>
+        <v>1.31</v>
       </c>
       <c r="L23" s="6">
         <f t="shared" si="15"/>
-        <v>13.82</v>
+        <v>1.31</v>
       </c>
       <c r="M23" s="6">
         <f t="shared" si="16"/>
-        <v>13.8</v>
-      </c>
-      <c r="N23" s="18"/>
-      <c r="O23" s="24" t="str">
+        <v>1.31</v>
+      </c>
+      <c r="N23" s="17"/>
+      <c r="O23" s="23" t="str">
         <f t="shared" si="17"/>
-        <v>1,A123185-ND</v>
-      </c>
-      <c r="P23" s="23" t="str">
+        <v>1,WM1814-ND</v>
+      </c>
+      <c r="P23" s="22" t="str">
         <f t="shared" si="18"/>
-        <v>571-7-967288-1|1</v>
+        <v>538-43045-0400|1</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="16.5" thickBot="1">
       <c r="A24" s="12">
         <v>1</v>
       </c>
-      <c r="B24" s="30" t="s">
-        <v>191</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>192</v>
+      <c r="B24" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>153</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>193</v>
+        <v>149</v>
       </c>
       <c r="E24" s="3"/>
-      <c r="F24" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="G24" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>195</v>
-      </c>
-      <c r="I24" s="17" t="s">
-        <v>196</v>
+      <c r="F24" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>150</v>
       </c>
       <c r="J24" s="5">
-        <v>1.31</v>
+        <v>3.7</v>
       </c>
       <c r="K24" s="5">
-        <v>1.31</v>
+        <v>3.22</v>
       </c>
       <c r="L24" s="6">
         <f t="shared" si="15"/>
-        <v>1.31</v>
+        <v>3.7</v>
       </c>
       <c r="M24" s="6">
         <f t="shared" si="16"/>
-        <v>1.31</v>
-      </c>
-      <c r="N24" s="18"/>
-      <c r="O24" s="24" t="str">
+        <v>3.22</v>
+      </c>
+      <c r="N24" s="17"/>
+      <c r="O24" s="23" t="str">
         <f t="shared" si="17"/>
-        <v>1,WM1814-ND</v>
-      </c>
-      <c r="P24" s="23" t="str">
+        <v>1,WM4723-ND</v>
+      </c>
+      <c r="P24" s="22" t="str">
         <f t="shared" si="18"/>
-        <v>538-43045-0400|1</v>
+        <v>538-43045-1400|1</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="16.5" thickBot="1">
       <c r="A25" s="12">
         <v>1</v>
       </c>
-      <c r="B25" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>159</v>
+      <c r="B25" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>154</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="G25" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="H25" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="I25" s="17" t="s">
-        <v>156</v>
+        <v>133</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="G25" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="J25" s="5">
-        <v>3.7</v>
+        <v>0.33</v>
       </c>
       <c r="K25" s="5">
-        <v>3.22</v>
+        <v>0.38</v>
       </c>
       <c r="L25" s="6">
         <f t="shared" si="15"/>
-        <v>3.7</v>
+        <v>0.33</v>
       </c>
       <c r="M25" s="6">
         <f t="shared" si="16"/>
-        <v>3.22</v>
-      </c>
-      <c r="N25" s="18"/>
-      <c r="O25" s="24" t="str">
+        <v>0.38</v>
+      </c>
+      <c r="N25" s="4"/>
+      <c r="O25" s="23" t="str">
         <f t="shared" si="17"/>
-        <v>1,WM4723-ND</v>
-      </c>
-      <c r="P25" s="23" t="str">
+        <v>1,WM3702-ND</v>
+      </c>
+      <c r="P25" s="22" t="str">
         <f t="shared" si="18"/>
-        <v>538-43045-1400|1</v>
+        <v>538-39-01-2060|1</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="16.5" thickBot="1">
       <c r="A26" s="12">
         <v>1</v>
       </c>
-      <c r="B26" s="30" t="s">
-        <v>145</v>
-      </c>
-      <c r="C26" s="20" t="s">
-        <v>160</v>
+      <c r="B26" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>148</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="F26" s="20" t="s">
-        <v>140</v>
+        <v>155</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="G26" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="H26" s="20" t="s">
-        <v>142</v>
+        <v>156</v>
+      </c>
+      <c r="H26" s="19" t="s">
+        <v>158</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="J26" s="5">
-        <v>0.33</v>
+        <v>0.79</v>
       </c>
       <c r="K26" s="5">
-        <v>0.38</v>
+        <v>0.79</v>
       </c>
       <c r="L26" s="6">
         <f t="shared" si="15"/>
-        <v>0.33</v>
+        <v>0.79</v>
       </c>
       <c r="M26" s="6">
         <f t="shared" si="16"/>
-        <v>0.38</v>
-      </c>
-      <c r="N26" s="4"/>
-      <c r="O26" s="24" t="str">
+        <v>0.79</v>
+      </c>
+      <c r="N26" s="17"/>
+      <c r="O26" s="21" t="str">
         <f t="shared" si="17"/>
-        <v>1,WM3702-ND</v>
-      </c>
-      <c r="P26" s="23" t="str">
+        <v>1,WM2489-ND</v>
+      </c>
+      <c r="P26" s="22" t="str">
         <f t="shared" si="18"/>
-        <v>538-39-01-2060|1</v>
+        <v>538-43025-1400|1</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="16.5" thickBot="1">
       <c r="A27" s="12">
-        <v>1</v>
-      </c>
-      <c r="B27" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>154</v>
+        <v>15</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>160</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>161</v>
       </c>
       <c r="E27" s="3"/>
-      <c r="F27" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="G27" s="33" t="s">
+      <c r="F27" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="G27" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="H27" s="20" t="s">
+      <c r="H27" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="I27" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="I27" s="2" t="s">
-        <v>163</v>
-      </c>
       <c r="J27" s="5">
-        <v>0.79</v>
+        <v>0.16</v>
       </c>
       <c r="K27" s="5">
-        <v>0.79</v>
+        <v>0.18</v>
       </c>
       <c r="L27" s="6">
         <f t="shared" si="15"/>
-        <v>0.79</v>
+        <v>2.4</v>
       </c>
       <c r="M27" s="6">
         <f t="shared" si="16"/>
-        <v>0.79</v>
-      </c>
-      <c r="N27" s="18"/>
-      <c r="O27" s="22" t="str">
-        <f t="shared" si="17"/>
-        <v>1,WM2489-ND</v>
-      </c>
-      <c r="P27" s="23" t="str">
-        <f t="shared" si="18"/>
-        <v>538-43025-1400|1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="16.5" thickBot="1">
-      <c r="A28" s="12">
-        <v>15</v>
-      </c>
-      <c r="B28" s="30" t="s">
-        <v>165</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>166</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>167</v>
-      </c>
+        <v>2.6999999999999997</v>
+      </c>
+      <c r="N27" s="17"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="22"/>
+    </row>
+    <row r="28" spans="1:16" ht="26.25" thickBot="1">
+      <c r="A28" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="G28" s="21" t="s">
-        <v>168</v>
-      </c>
-      <c r="H28" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="J28" s="5">
-        <v>0.16</v>
-      </c>
-      <c r="K28" s="5">
-        <v>0.18</v>
-      </c>
-      <c r="L28" s="6">
-        <f t="shared" si="15"/>
-        <v>2.4</v>
-      </c>
-      <c r="M28" s="6">
-        <f t="shared" si="16"/>
-        <v>2.6999999999999997</v>
-      </c>
-      <c r="N28" s="18"/>
-      <c r="O28" s="22"/>
-      <c r="P28" s="23"/>
-    </row>
-    <row r="29" spans="1:16" ht="26.25" thickBot="1">
-      <c r="A29" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="B29" s="4"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="22"/>
+    </row>
+    <row r="29" spans="1:16" ht="18" customHeight="1" thickBot="1">
+      <c r="A29" s="12">
+        <v>1</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
+      <c r="D29" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="G29" s="20"/>
+      <c r="H29" s="16"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
-      <c r="N29" s="18"/>
-      <c r="O29" s="22"/>
-      <c r="P29" s="23"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="22"/>
     </row>
     <row r="30" spans="1:16" ht="18" customHeight="1" thickBot="1">
       <c r="A30" s="12">
         <v>1</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="F30" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="G30" s="21"/>
-      <c r="H30" s="17"/>
+        <v>130</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="G30" s="20"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="22"/>
-      <c r="P30" s="23"/>
-    </row>
-    <row r="31" spans="1:16" ht="18" customHeight="1" thickBot="1">
+      <c r="N30" s="17"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="22"/>
+    </row>
+    <row r="31" spans="1:16" ht="16.5" thickBot="1">
       <c r="A31" s="12">
         <v>1</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="F31" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="G31" s="21"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
+        <v>123</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="G31" s="20"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
-      <c r="N31" s="18"/>
-      <c r="O31" s="22"/>
-      <c r="P31" s="23"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="22"/>
     </row>
     <row r="32" spans="1:16" ht="16.5" thickBot="1">
-      <c r="A32" s="12">
-        <v>1</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>126</v>
-      </c>
+      <c r="A32" s="10"/>
+      <c r="B32" s="4"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="F32" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="G32" s="21"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="18"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" s="36"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K32" s="1"/>
+      <c r="L32" s="8">
+        <f>SUM(L2:L21)</f>
+        <v>37.700000000000003</v>
+      </c>
+      <c r="M32" s="8">
+        <f>SUM(M2:M21)</f>
+        <v>38.409999999999997</v>
+      </c>
+      <c r="N32" s="18" t="s">
+        <v>11</v>
+      </c>
       <c r="O32" s="22"/>
-      <c r="P32" s="23"/>
-    </row>
-    <row r="33" spans="1:16" ht="16.5" thickBot="1">
-      <c r="A33" s="10"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H33" s="37"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K33" s="1"/>
-      <c r="L33" s="8">
-        <f>SUM(L2:L22)</f>
-        <v>37.900000000000006</v>
-      </c>
-      <c r="M33" s="8">
-        <f>SUM(M2:M22)</f>
-        <v>38.61</v>
-      </c>
-      <c r="N33" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="O33" s="23"/>
-      <c r="P33" s="23"/>
-    </row>
-    <row r="34" spans="1:16" ht="16.5" customHeight="1"/>
+      <c r="P32" s="22"/>
+    </row>
+    <row r="33" ht="16.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G32:H32"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>